<commit_message>
12:26 fixat long winning animation i 2 versioner
</commit_message>
<xml_diff>
--- a/Grafik/Administrativt/Grafikplanering-SGA.xlsx
+++ b/Grafik/Administrativt/Grafikplanering-SGA.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>Vecka:</t>
   </si>
@@ -588,7 +588,7 @@
   <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -797,7 +797,9 @@
       <c r="F14" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">

</xml_diff>